<commit_message>
Add key-based hotel price updater with auto mode and snapshot dates - Added hotel_keys_db.json with 149 PRTC hotels mapped to Xotelo keys - Refactored xotelo_price_updater.py for direct key lookups - Added --auto mode for monthly automation - Added snapshot date column in Excel output - Added extract_all_hotels.py for API hotel extraction - Added key_manager.py and templates for key management
</commit_message>
<xml_diff>
--- a/PRTC Endorsed Hotels - Updated Xotelo.xlsx
+++ b/PRTC Endorsed Hotels - Updated Xotelo.xlsx
@@ -955,7 +955,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:M153"/>
+  <dimension ref="A1:K153"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1013,16 +1013,6 @@
       </c>
       <c r="K1" s="3" t="inlineStr">
         <is>
-          <t>API_Match_Name</t>
-        </is>
-      </c>
-      <c r="L1" s="3" t="inlineStr">
-        <is>
-          <t>Match_Score</t>
-        </is>
-      </c>
-      <c r="M1" s="3" t="inlineStr">
-        <is>
           <t>Hotel_Key</t>
         </is>
       </c>
@@ -1056,20 +1046,10 @@
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K2" t="inlineStr">
-        <is>
-          <t>The St. Regis Bahia Beach Resort, Puerto Rico</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>72%</t>
-        </is>
-      </c>
-      <c r="M2" t="inlineStr">
         <is>
           <t>g147319-d1837036</t>
         </is>
@@ -1104,7 +1084,7 @@
       </c>
       <c r="H3" s="1" t="n"/>
       <c r="I3" t="n">
-        <v>3856</v>
+        <v>3654</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -1112,16 +1092,6 @@
         </is>
       </c>
       <c r="K3" t="inlineStr">
-        <is>
-          <t>Dorado Beach, a Ritz-Carlton Reserve</t>
-        </is>
-      </c>
-      <c r="L3" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M3" t="inlineStr">
         <is>
           <t>g147319-d3518813</t>
         </is>
@@ -1156,20 +1126,10 @@
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K4" t="inlineStr">
-        <is>
-          <t>Condado Vanderbilt Hotel</t>
-        </is>
-      </c>
-      <c r="L4" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M4" t="inlineStr">
         <is>
           <t>g147319-d6691692</t>
         </is>
@@ -1212,16 +1172,6 @@
       </c>
       <c r="K5" t="inlineStr">
         <is>
-          <t>San Juan Marriott Resort &amp; Stellaris Casino</t>
-        </is>
-      </c>
-      <c r="L5" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M5" t="inlineStr">
-        <is>
           <t>g147319-d149920</t>
         </is>
       </c>
@@ -1255,7 +1205,12 @@
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>g147322-d3877676</t>
         </is>
       </c>
     </row>
@@ -1288,20 +1243,10 @@
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K7" t="inlineStr">
-        <is>
-          <t>Royal Isabela</t>
-        </is>
-      </c>
-      <c r="L7" t="inlineStr">
-        <is>
-          <t>68%</t>
-        </is>
-      </c>
-      <c r="M7" t="inlineStr">
         <is>
           <t>g147319-d3333177</t>
         </is>
@@ -1335,7 +1280,7 @@
         <v>202512</v>
       </c>
       <c r="I8" t="n">
-        <v>372</v>
+        <v>421</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -1343,16 +1288,6 @@
         </is>
       </c>
       <c r="K8" t="inlineStr">
-        <is>
-          <t>El Conquistador Resort</t>
-        </is>
-      </c>
-      <c r="L8" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M8" t="inlineStr">
         <is>
           <t>g147319-d148045</t>
         </is>
@@ -1395,16 +1330,6 @@
       </c>
       <c r="K9" t="inlineStr">
         <is>
-          <t>Sheraton Puerto Rico Resort And Casino</t>
-        </is>
-      </c>
-      <c r="L9" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M9" t="inlineStr">
-        <is>
           <t>g147319-d1423064</t>
         </is>
       </c>
@@ -1446,16 +1371,6 @@
       </c>
       <c r="K10" t="inlineStr">
         <is>
-          <t>Fairmont El San Juan Hotel</t>
-        </is>
-      </c>
-      <c r="L10" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M10" t="inlineStr">
-        <is>
           <t>g147319-d155800</t>
         </is>
       </c>
@@ -1497,16 +1412,6 @@
       </c>
       <c r="K11" t="inlineStr">
         <is>
-          <t>Royal Sonesta</t>
-        </is>
-      </c>
-      <c r="L11" t="inlineStr">
-        <is>
-          <t>74%</t>
-        </is>
-      </c>
-      <c r="M11" t="inlineStr">
-        <is>
           <t>g147319-d150446</t>
         </is>
       </c>
@@ -1540,20 +1445,10 @@
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K12" t="inlineStr">
-        <is>
-          <t>Villa Montana Beach Resort</t>
-        </is>
-      </c>
-      <c r="L12" t="inlineStr">
-        <is>
-          <t>95%</t>
-        </is>
-      </c>
-      <c r="M12" t="inlineStr">
         <is>
           <t>g147319-d224196</t>
         </is>
@@ -1587,7 +1482,7 @@
         <v>202512</v>
       </c>
       <c r="I13" t="n">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1595,16 +1490,6 @@
         </is>
       </c>
       <c r="K13" t="inlineStr">
-        <is>
-          <t>O:LV Fifty Five</t>
-        </is>
-      </c>
-      <c r="L13" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M13" t="inlineStr">
         <is>
           <t>g147319-d13969946</t>
         </is>
@@ -1638,7 +1523,7 @@
         <v>202512</v>
       </c>
       <c r="I14" t="n">
-        <v>362</v>
+        <v>342</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1646,16 +1531,6 @@
         </is>
       </c>
       <c r="K14" t="inlineStr">
-        <is>
-          <t>Embassy Suites by Hilton Dorado del Mar Beach Resort</t>
-        </is>
-      </c>
-      <c r="L14" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M14" t="inlineStr">
         <is>
           <t>g147319-d209618</t>
         </is>
@@ -1690,20 +1565,10 @@
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K15" t="inlineStr">
-        <is>
-          <t>Hyatt Place San Juan</t>
-        </is>
-      </c>
-      <c r="L15" t="inlineStr">
-        <is>
-          <t>64%</t>
-        </is>
-      </c>
-      <c r="M15" t="inlineStr">
         <is>
           <t>g147319-d9602805</t>
         </is>
@@ -1737,24 +1602,14 @@
         <v>202512</v>
       </c>
       <c r="I16" t="n">
-        <v>730</v>
+        <v>748</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>Trip.com</t>
+          <t>Agoda.com</t>
         </is>
       </c>
       <c r="K16" t="inlineStr">
-        <is>
-          <t>Wyndham Grand Rio Mar Rainforest Beach &amp; Golf Resort</t>
-        </is>
-      </c>
-      <c r="L16" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M16" t="inlineStr">
         <is>
           <t>g147319-d148598</t>
         </is>
@@ -1787,25 +1642,12 @@
       <c r="F17" t="n">
         <v>202512</v>
       </c>
-      <c r="I17" t="n">
-        <v>335</v>
-      </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>Copamarina Beach</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K17" t="inlineStr">
-        <is>
-          <t>Copamarina Beach Resort &amp; Spa</t>
-        </is>
-      </c>
-      <c r="L17" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M17" t="inlineStr">
         <is>
           <t>g147319-d148807</t>
         </is>
@@ -1839,7 +1681,7 @@
         <v>202512</v>
       </c>
       <c r="I18" t="n">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1847,16 +1689,6 @@
         </is>
       </c>
       <c r="K18" t="inlineStr">
-        <is>
-          <t>Condado Ocean Club</t>
-        </is>
-      </c>
-      <c r="L18" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M18" t="inlineStr">
         <is>
           <t>g147319-d12522646</t>
         </is>
@@ -1890,7 +1722,7 @@
         <v>202512</v>
       </c>
       <c r="I19" t="n">
-        <v>554</v>
+        <v>567</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1898,16 +1730,6 @@
         </is>
       </c>
       <c r="K19" t="inlineStr">
-        <is>
-          <t>Olive Boutique Hotel</t>
-        </is>
-      </c>
-      <c r="L19" t="inlineStr">
-        <is>
-          <t>97%</t>
-        </is>
-      </c>
-      <c r="M19" t="inlineStr">
         <is>
           <t>g147319-d3152780</t>
         </is>
@@ -1941,24 +1763,14 @@
         <v>202512</v>
       </c>
       <c r="I20" t="n">
-        <v>493</v>
+        <v>479</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>Booking.com</t>
+          <t>Agoda.com</t>
         </is>
       </c>
       <c r="K20" t="inlineStr">
-        <is>
-          <t>The Condado Plaza Hotel</t>
-        </is>
-      </c>
-      <c r="L20" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M20" t="inlineStr">
         <is>
           <t>g147319-d150443</t>
         </is>
@@ -1992,7 +1804,7 @@
         <v>202512</v>
       </c>
       <c r="I21" t="n">
-        <v>571</v>
+        <v>658</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -2000,16 +1812,6 @@
         </is>
       </c>
       <c r="K21" t="inlineStr">
-        <is>
-          <t>Hyatt Regency Grand Reserve Puerto Rico</t>
-        </is>
-      </c>
-      <c r="L21" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M21" t="inlineStr">
         <is>
           <t>g147319-d284987</t>
         </is>
@@ -2052,16 +1854,6 @@
       </c>
       <c r="K22" t="inlineStr">
         <is>
-          <t>Casa Costera, Isla Verde Beach, Apartments By Marriott Bonvoy</t>
-        </is>
-      </c>
-      <c r="L22" t="inlineStr">
-        <is>
-          <t>83%</t>
-        </is>
-      </c>
-      <c r="M22" t="inlineStr">
-        <is>
           <t>g147319-d26878084</t>
         </is>
       </c>
@@ -2095,20 +1887,10 @@
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K23" t="inlineStr">
-        <is>
-          <t>Embassy Suites by Hilton San Juan Hotel &amp; Casino</t>
-        </is>
-      </c>
-      <c r="L23" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M23" t="inlineStr">
         <is>
           <t>g147319-d151713</t>
         </is>
@@ -2151,16 +1933,6 @@
       </c>
       <c r="K24" t="inlineStr">
         <is>
-          <t>Mayagüez Resort &amp; Casino</t>
-        </is>
-      </c>
-      <c r="L24" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M24" t="inlineStr">
-        <is>
           <t>g147319-d297785</t>
         </is>
       </c>
@@ -2193,7 +1965,7 @@
         <v>202512</v>
       </c>
       <c r="I25" t="n">
-        <v>578</v>
+        <v>557</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -2201,16 +1973,6 @@
         </is>
       </c>
       <c r="K25" t="inlineStr">
-        <is>
-          <t>Condado Palm Inn San Juan, Tapestry Collection by Hilton</t>
-        </is>
-      </c>
-      <c r="L25" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M25" t="inlineStr">
         <is>
           <t>g147319-d242220</t>
         </is>
@@ -2244,24 +2006,14 @@
         <v>202512</v>
       </c>
       <c r="I26" t="n">
-        <v>694</v>
+        <v>628</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>Booking.com</t>
+          <t>Trip.com</t>
         </is>
       </c>
       <c r="K26" t="inlineStr">
-        <is>
-          <t>Courtyard by Marriott Isla Verde Beach Resort</t>
-        </is>
-      </c>
-      <c r="L26" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M26" t="inlineStr">
         <is>
           <t>g147319-d268430</t>
         </is>
@@ -2296,20 +2048,10 @@
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K27" t="inlineStr">
-        <is>
-          <t>Margaritaville Vacation Club At Wyndham Rio Mar</t>
-        </is>
-      </c>
-      <c r="L27" t="inlineStr">
-        <is>
-          <t>96%</t>
-        </is>
-      </c>
-      <c r="M27" t="inlineStr">
         <is>
           <t>g147319-d16659689</t>
         </is>
@@ -2344,7 +2086,12 @@
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>g147320-d2179878</t>
         </is>
       </c>
     </row>
@@ -2376,7 +2123,7 @@
         <v>202512</v>
       </c>
       <c r="I29" t="n">
-        <v>598</v>
+        <v>479</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -2384,16 +2131,6 @@
         </is>
       </c>
       <c r="K29" t="inlineStr">
-        <is>
-          <t>DoubleTree by Hilton Hotel San Juan</t>
-        </is>
-      </c>
-      <c r="L29" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M29" t="inlineStr">
         <is>
           <t>g147319-d151682</t>
         </is>
@@ -2426,9 +2163,17 @@
       <c r="F30" t="n">
         <v>202512</v>
       </c>
+      <c r="I30" t="n">
+        <v>769</v>
+      </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>Agoda.com</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>g147320-d26857069</t>
         </is>
       </c>
     </row>
@@ -2461,7 +2206,12 @@
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>g264369-d151980</t>
         </is>
       </c>
     </row>
@@ -2493,7 +2243,7 @@
         <v>202512</v>
       </c>
       <c r="I32" t="n">
-        <v>550</v>
+        <v>584</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -2501,16 +2251,6 @@
         </is>
       </c>
       <c r="K32" t="inlineStr">
-        <is>
-          <t>AC Hotel San Juan Condado</t>
-        </is>
-      </c>
-      <c r="L32" t="inlineStr">
-        <is>
-          <t>76%</t>
-        </is>
-      </c>
-      <c r="M32" t="inlineStr">
         <is>
           <t>g147319-d12349375</t>
         </is>
@@ -2545,20 +2285,10 @@
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K33" t="inlineStr">
-        <is>
-          <t>Decanter Hotel</t>
-        </is>
-      </c>
-      <c r="L33" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M33" t="inlineStr">
         <is>
           <t>g147319-d8618734</t>
         </is>
@@ -2591,25 +2321,12 @@
       <c r="F34" t="n">
         <v>202512</v>
       </c>
-      <c r="I34" t="n">
-        <v>405</v>
-      </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>Trip.com</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K34" t="inlineStr">
-        <is>
-          <t>Caribe Hilton Hotel</t>
-        </is>
-      </c>
-      <c r="L34" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M34" t="inlineStr">
         <is>
           <t>g147319-d149921</t>
         </is>
@@ -2644,20 +2361,10 @@
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K35" t="inlineStr">
-        <is>
-          <t>Rincon Beach Resort</t>
-        </is>
-      </c>
-      <c r="L35" t="inlineStr">
-        <is>
-          <t>92%</t>
-        </is>
-      </c>
-      <c r="M35" t="inlineStr">
         <is>
           <t>g147319-d242226</t>
         </is>
@@ -2700,16 +2407,6 @@
       </c>
       <c r="K36" t="inlineStr">
         <is>
-          <t>Boho Beach Club</t>
-        </is>
-      </c>
-      <c r="L36" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M36" t="inlineStr">
-        <is>
           <t>g147319-d13324163</t>
         </is>
       </c>
@@ -2743,7 +2440,12 @@
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>g147320-d23130157</t>
         </is>
       </c>
     </row>
@@ -2776,20 +2478,10 @@
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K38" t="inlineStr">
-        <is>
-          <t>Rincon Of The Seas Grand Caribbean Hotel</t>
-        </is>
-      </c>
-      <c r="L38" t="inlineStr">
-        <is>
-          <t>97%</t>
-        </is>
-      </c>
-      <c r="M38" t="inlineStr">
         <is>
           <t>g147319-d264386</t>
         </is>
@@ -2832,16 +2524,6 @@
       </c>
       <c r="K39" t="inlineStr">
         <is>
-          <t>Residence Inn by Marriott San Juan Isla Verde</t>
-        </is>
-      </c>
-      <c r="L39" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M39" t="inlineStr">
-        <is>
           <t>g147319-d23924461</t>
         </is>
       </c>
@@ -2873,11 +2555,6 @@
       <c r="F40" t="n">
         <v>202512</v>
       </c>
-      <c r="J40" t="inlineStr">
-        <is>
-          <t>Not found</t>
-        </is>
-      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -2908,20 +2585,10 @@
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K41" t="inlineStr">
-        <is>
-          <t>EL Yunque Rainforest Inn</t>
-        </is>
-      </c>
-      <c r="L41" t="inlineStr">
-        <is>
-          <t>74%</t>
-        </is>
-      </c>
-      <c r="M41" t="inlineStr">
         <is>
           <t>g147319-d503287</t>
         </is>
@@ -2955,24 +2622,14 @@
         <v>202512</v>
       </c>
       <c r="I42" t="n">
-        <v>380</v>
+        <v>333</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>Agoda.com</t>
+          <t>Trip.com</t>
         </is>
       </c>
       <c r="K42" t="inlineStr">
-        <is>
-          <t>Wyndham Palmas Beach And Golf Boutique Resort</t>
-        </is>
-      </c>
-      <c r="L42" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M42" t="inlineStr">
         <is>
           <t>g147319-d310451</t>
         </is>
@@ -3006,24 +2663,14 @@
         <v>202512</v>
       </c>
       <c r="I43" t="n">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>Vio.com</t>
+          <t>Agoda.com</t>
         </is>
       </c>
       <c r="K43" t="inlineStr">
-        <is>
-          <t>Aquarius Vacation Club at Dorado del Mar</t>
-        </is>
-      </c>
-      <c r="L43" t="inlineStr">
-        <is>
-          <t>79%</t>
-        </is>
-      </c>
-      <c r="M43" t="inlineStr">
         <is>
           <t>g147319-d1232094</t>
         </is>
@@ -3066,16 +2713,6 @@
       </c>
       <c r="K44" t="inlineStr">
         <is>
-          <t>Four Points by Sheraton Caguas Real Hotel &amp; Casino</t>
-        </is>
-      </c>
-      <c r="L44" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M44" t="inlineStr">
-        <is>
           <t>g147319-d534897</t>
         </is>
       </c>
@@ -3117,16 +2754,6 @@
       </c>
       <c r="K45" t="inlineStr">
         <is>
-          <t>Hotel El Convento</t>
-        </is>
-      </c>
-      <c r="L45" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M45" t="inlineStr">
-        <is>
           <t>g147319-d148043</t>
         </is>
       </c>
@@ -3159,24 +2786,14 @@
         <v>202512</v>
       </c>
       <c r="I46" t="n">
-        <v>129</v>
+        <v>134</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>Vio.com</t>
+          <t>Agoda.com</t>
         </is>
       </c>
       <c r="K46" t="inlineStr">
-        <is>
-          <t>Aquarius Vacation Club at Dorado del Mar</t>
-        </is>
-      </c>
-      <c r="L46" t="inlineStr">
-        <is>
-          <t>70%</t>
-        </is>
-      </c>
-      <c r="M46" t="inlineStr">
         <is>
           <t>g147319-d1232094</t>
         </is>
@@ -3211,20 +2828,10 @@
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K47" t="inlineStr">
-        <is>
-          <t>Hyatt Vacation Club At Hacienda del Mar</t>
-        </is>
-      </c>
-      <c r="L47" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M47" t="inlineStr">
         <is>
           <t>g147319-d254380</t>
         </is>
@@ -3267,16 +2874,6 @@
       </c>
       <c r="K48" t="inlineStr">
         <is>
-          <t>Courtyard by Marriott Aguadilla</t>
-        </is>
-      </c>
-      <c r="L48" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M48" t="inlineStr">
-        <is>
           <t>g147319-d858414</t>
         </is>
       </c>
@@ -3309,7 +2906,7 @@
         <v>202512</v>
       </c>
       <c r="I49" t="n">
-        <v>283</v>
+        <v>261</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
@@ -3317,16 +2914,6 @@
         </is>
       </c>
       <c r="K49" t="inlineStr">
-        <is>
-          <t>TRYP by Wyndham Isla Verde</t>
-        </is>
-      </c>
-      <c r="L49" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M49" t="inlineStr">
         <is>
           <t>g147319-d151806</t>
         </is>
@@ -3360,7 +2947,7 @@
         <v>202512</v>
       </c>
       <c r="I50" t="n">
-        <v>256</v>
+        <v>274</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
@@ -3368,16 +2955,6 @@
         </is>
       </c>
       <c r="K50" t="inlineStr">
-        <is>
-          <t>Hilton Ponce Golf &amp; Casino Resort</t>
-        </is>
-      </c>
-      <c r="L50" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M50" t="inlineStr">
         <is>
           <t>g147319-d151671</t>
         </is>
@@ -3411,7 +2988,7 @@
         <v>202512</v>
       </c>
       <c r="I51" t="n">
-        <v>330</v>
+        <v>364</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
@@ -3419,16 +2996,6 @@
         </is>
       </c>
       <c r="K51" t="inlineStr">
-        <is>
-          <t>Fairfield By Marriott Luquillo Beach</t>
-        </is>
-      </c>
-      <c r="L51" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M51" t="inlineStr">
         <is>
           <t>g147319-d26627285</t>
         </is>
@@ -3471,16 +3038,6 @@
       </c>
       <c r="K52" t="inlineStr">
         <is>
-          <t>Hyatt Place Bayamón</t>
-        </is>
-      </c>
-      <c r="L52" t="inlineStr">
-        <is>
-          <t>67%</t>
-        </is>
-      </c>
-      <c r="M52" t="inlineStr">
-        <is>
           <t>g147319-d5274354</t>
         </is>
       </c>
@@ -3513,7 +3070,7 @@
         <v>202512</v>
       </c>
       <c r="I53" t="n">
-        <v>568</v>
+        <v>641</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
@@ -3521,16 +3078,6 @@
         </is>
       </c>
       <c r="K53" t="inlineStr">
-        <is>
-          <t>Aire De O:live</t>
-        </is>
-      </c>
-      <c r="L53" t="inlineStr">
-        <is>
-          <t>91%</t>
-        </is>
-      </c>
-      <c r="M53" t="inlineStr">
         <is>
           <t>g147319-d30767613</t>
         </is>
@@ -3564,7 +3111,7 @@
         <v>202512</v>
       </c>
       <c r="I54" t="n">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
@@ -3572,16 +3119,6 @@
         </is>
       </c>
       <c r="K54" t="inlineStr">
-        <is>
-          <t>Punta Borinquen Resort</t>
-        </is>
-      </c>
-      <c r="L54" t="inlineStr">
-        <is>
-          <t>75%</t>
-        </is>
-      </c>
-      <c r="M54" t="inlineStr">
         <is>
           <t>g147319-d12220946</t>
         </is>
@@ -3616,20 +3153,10 @@
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K55" t="inlineStr">
-        <is>
-          <t>Hilton Garden Inn San Juan Condado</t>
-        </is>
-      </c>
-      <c r="L55" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M55" t="inlineStr">
         <is>
           <t>g147319-d26555257</t>
         </is>
@@ -3664,20 +3191,10 @@
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K56" t="inlineStr">
-        <is>
-          <t>Hyatt Place San Juan</t>
-        </is>
-      </c>
-      <c r="L56" t="inlineStr">
-        <is>
-          <t>77%</t>
-        </is>
-      </c>
-      <c r="M56" t="inlineStr">
         <is>
           <t>g147319-d9602805</t>
         </is>
@@ -3712,20 +3229,10 @@
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K57" t="inlineStr">
-        <is>
-          <t>Club Seabourne Hotel</t>
-        </is>
-      </c>
-      <c r="L57" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M57" t="inlineStr">
         <is>
           <t>g147319-d151840</t>
         </is>
@@ -3760,20 +3267,10 @@
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K58" t="inlineStr">
-        <is>
-          <t>Fajardo Inn Resort</t>
-        </is>
-      </c>
-      <c r="L58" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M58" t="inlineStr">
         <is>
           <t>g147319-d155796</t>
         </is>
@@ -3808,7 +3305,12 @@
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>g147326-d1569786</t>
         </is>
       </c>
     </row>
@@ -3840,7 +3342,7 @@
         <v>202512</v>
       </c>
       <c r="I60" t="n">
-        <v>152</v>
+        <v>179</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
@@ -3848,16 +3350,6 @@
         </is>
       </c>
       <c r="K60" t="inlineStr">
-        <is>
-          <t>Holiday Inn Mayaguez &amp; Tropical Casino by IHG</t>
-        </is>
-      </c>
-      <c r="L60" t="inlineStr">
-        <is>
-          <t>92%</t>
-        </is>
-      </c>
-      <c r="M60" t="inlineStr">
         <is>
           <t>g147319-d151796</t>
         </is>
@@ -3891,7 +3383,7 @@
         <v>202512</v>
       </c>
       <c r="I61" t="n">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
@@ -3899,16 +3391,6 @@
         </is>
       </c>
       <c r="K61" t="inlineStr">
-        <is>
-          <t>TRYP by Wyndham Mayaguez</t>
-        </is>
-      </c>
-      <c r="L61" t="inlineStr">
-        <is>
-          <t>96%</t>
-        </is>
-      </c>
-      <c r="M61" t="inlineStr">
         <is>
           <t>g147319-d24800269</t>
         </is>
@@ -3941,22 +3423,15 @@
       <c r="F62" t="n">
         <v>202512</v>
       </c>
+      <c r="I62" t="n">
+        <v>446</v>
+      </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>Courtyard</t>
         </is>
       </c>
       <c r="K62" t="inlineStr">
-        <is>
-          <t>Courtyard San Juan Miramar</t>
-        </is>
-      </c>
-      <c r="L62" t="inlineStr">
-        <is>
-          <t>81%</t>
-        </is>
-      </c>
-      <c r="M62" t="inlineStr">
         <is>
           <t>g147319-d600604</t>
         </is>
@@ -3990,7 +3465,7 @@
         <v>202512</v>
       </c>
       <c r="I63" t="n">
-        <v>688</v>
+        <v>530</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
@@ -3998,16 +3473,6 @@
         </is>
       </c>
       <c r="K63" t="inlineStr">
-        <is>
-          <t>Hampton Inn &amp; Suites San Juan</t>
-        </is>
-      </c>
-      <c r="L63" t="inlineStr">
-        <is>
-          <t>76%</t>
-        </is>
-      </c>
-      <c r="M63" t="inlineStr">
         <is>
           <t>g147319-d150241</t>
         </is>
@@ -4042,20 +3507,10 @@
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K64" t="inlineStr">
-        <is>
-          <t>Hotel Miramar</t>
-        </is>
-      </c>
-      <c r="L64" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M64" t="inlineStr">
         <is>
           <t>g147319-d253693</t>
         </is>
@@ -4090,20 +3545,10 @@
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K65" t="inlineStr">
-        <is>
-          <t>Hyatt House San Juan</t>
-        </is>
-      </c>
-      <c r="L65" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M65" t="inlineStr">
         <is>
           <t>g147319-d6892975</t>
         </is>
@@ -4146,16 +3591,6 @@
       </c>
       <c r="K66" t="inlineStr">
         <is>
-          <t>Hyatt Place Manati</t>
-        </is>
-      </c>
-      <c r="L66" t="inlineStr">
-        <is>
-          <t>68%</t>
-        </is>
-      </c>
-      <c r="M66" t="inlineStr">
-        <is>
           <t>g147319-d5598171</t>
         </is>
       </c>
@@ -4189,20 +3624,10 @@
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K67" t="inlineStr">
-        <is>
-          <t>Corcega Beachfront Suites</t>
-        </is>
-      </c>
-      <c r="L67" t="inlineStr">
-        <is>
-          <t>71%</t>
-        </is>
-      </c>
-      <c r="M67" t="inlineStr">
         <is>
           <t>g147319-d26629555</t>
         </is>
@@ -4237,20 +3662,10 @@
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K68" t="inlineStr">
-        <is>
-          <t>Aqua Marina Beach Club</t>
-        </is>
-      </c>
-      <c r="L68" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M68" t="inlineStr">
         <is>
           <t>g147319-d623904</t>
         </is>
@@ -4293,16 +3708,6 @@
       </c>
       <c r="K69" t="inlineStr">
         <is>
-          <t>Don Rafa Boutique Hotel &amp; Residences</t>
-        </is>
-      </c>
-      <c r="L69" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M69" t="inlineStr">
-        <is>
           <t>g147319-d25178239</t>
         </is>
       </c>
@@ -4336,20 +3741,10 @@
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K70" t="inlineStr">
-        <is>
-          <t>Hotel Villa del Sol</t>
-        </is>
-      </c>
-      <c r="L70" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M70" t="inlineStr">
         <is>
           <t>g147319-d151808</t>
         </is>
@@ -4392,16 +3787,6 @@
       </c>
       <c r="K71" t="inlineStr">
         <is>
-          <t>Ponce Plaza Hotel &amp; Casino</t>
-        </is>
-      </c>
-      <c r="L71" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M71" t="inlineStr">
-        <is>
           <t>g147319-d6847423</t>
         </is>
       </c>
@@ -4434,7 +3819,7 @@
         <v>202512</v>
       </c>
       <c r="I72" t="n">
-        <v>353</v>
+        <v>362</v>
       </c>
       <c r="J72" t="inlineStr">
         <is>
@@ -4442,16 +3827,6 @@
         </is>
       </c>
       <c r="K72" t="inlineStr">
-        <is>
-          <t>La Terraza de San Juan</t>
-        </is>
-      </c>
-      <c r="L72" t="inlineStr">
-        <is>
-          <t>78%</t>
-        </is>
-      </c>
-      <c r="M72" t="inlineStr">
         <is>
           <t>g147319-d1988329</t>
         </is>
@@ -4485,7 +3860,7 @@
         <v>202512</v>
       </c>
       <c r="I73" t="n">
-        <v>278</v>
+        <v>294</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
@@ -4493,16 +3868,6 @@
         </is>
       </c>
       <c r="K73" t="inlineStr">
-        <is>
-          <t>The Wave Hotel Condado</t>
-        </is>
-      </c>
-      <c r="L73" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M73" t="inlineStr">
         <is>
           <t>g147319-d10195804</t>
         </is>
@@ -4537,20 +3902,10 @@
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K74" t="inlineStr">
-        <is>
-          <t>352 Guest House Hotel Boutique</t>
-        </is>
-      </c>
-      <c r="L74" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M74" t="inlineStr">
         <is>
           <t>g147319-d15141926</t>
         </is>
@@ -4583,9 +3938,17 @@
       <c r="F75" t="n">
         <v>202512</v>
       </c>
+      <c r="I75" t="n">
+        <v>524</v>
+      </c>
       <c r="J75" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>Trip.com</t>
+        </is>
+      </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>g147320-d249485</t>
         </is>
       </c>
     </row>
@@ -4626,16 +3989,6 @@
       </c>
       <c r="K76" t="inlineStr">
         <is>
-          <t>HiBird Apartment And Suites Hotel</t>
-        </is>
-      </c>
-      <c r="L76" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M76" t="inlineStr">
-        <is>
           <t>g147319-d25247369</t>
         </is>
       </c>
@@ -4669,20 +4022,10 @@
       </c>
       <c r="J77" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K77" t="inlineStr">
-        <is>
-          <t>Acacia Boutique Hotel</t>
-        </is>
-      </c>
-      <c r="L77" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M77" t="inlineStr">
         <is>
           <t>g147319-d151832</t>
         </is>
@@ -4715,22 +4058,15 @@
       <c r="F78" t="n">
         <v>202512</v>
       </c>
+      <c r="I78" t="n">
+        <v>196</v>
+      </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>Agoda.com</t>
         </is>
       </c>
       <c r="K78" t="inlineStr">
-        <is>
-          <t>San Juan Airport Hotel</t>
-        </is>
-      </c>
-      <c r="L78" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M78" t="inlineStr">
         <is>
           <t>g147319-d498911</t>
         </is>
@@ -4764,7 +4100,7 @@
         <v>202512</v>
       </c>
       <c r="I79" t="n">
-        <v>407</v>
+        <v>439</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
@@ -4772,16 +4108,6 @@
         </is>
       </c>
       <c r="K79" t="inlineStr">
-        <is>
-          <t>Aloft San Juan</t>
-        </is>
-      </c>
-      <c r="L79" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M79" t="inlineStr">
         <is>
           <t>g147319-d20116315</t>
         </is>
@@ -4815,24 +4141,14 @@
         <v>202512</v>
       </c>
       <c r="I80" t="n">
-        <v>199</v>
+        <v>224</v>
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t>Aloft.com</t>
+          <t>Trip.com</t>
         </is>
       </c>
       <c r="K80" t="inlineStr">
-        <is>
-          <t>Aloft Ponce Hotel &amp; Casino</t>
-        </is>
-      </c>
-      <c r="L80" t="inlineStr">
-        <is>
-          <t>76%</t>
-        </is>
-      </c>
-      <c r="M80" t="inlineStr">
         <is>
           <t>g147319-d21502214</t>
         </is>
@@ -4875,16 +4191,6 @@
       </c>
       <c r="K81" t="inlineStr">
         <is>
-          <t>Holiday Inn Ponce &amp; Tropical Casino by IHG</t>
-        </is>
-      </c>
-      <c r="L81" t="inlineStr">
-        <is>
-          <t>94%</t>
-        </is>
-      </c>
-      <c r="M81" t="inlineStr">
-        <is>
           <t>g147319-d151797</t>
         </is>
       </c>
@@ -4918,20 +4224,10 @@
       </c>
       <c r="J82" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K82" t="inlineStr">
-        <is>
-          <t>Casa de Amistad</t>
-        </is>
-      </c>
-      <c r="L82" t="inlineStr">
-        <is>
-          <t>73%</t>
-        </is>
-      </c>
-      <c r="M82" t="inlineStr">
         <is>
           <t>g147319-d280418</t>
         </is>
@@ -4964,25 +4260,12 @@
       <c r="F83" t="n">
         <v>202512</v>
       </c>
-      <c r="I83" t="n">
-        <v>335</v>
-      </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>Booking.com</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K83" t="inlineStr">
-        <is>
-          <t>Casa Wilson Inn</t>
-        </is>
-      </c>
-      <c r="L83" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M83" t="inlineStr">
         <is>
           <t>g147319-d17741745</t>
         </is>
@@ -5017,20 +4300,10 @@
       </c>
       <c r="J84" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K84" t="inlineStr">
-        <is>
-          <t>Parador Villas Del Mar Hau</t>
-        </is>
-      </c>
-      <c r="L84" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M84" t="inlineStr">
         <is>
           <t>g147319-d275180</t>
         </is>
@@ -5065,20 +4338,10 @@
       </c>
       <c r="J85" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K85" t="inlineStr">
-        <is>
-          <t>Hotel Puerto Valdes</t>
-        </is>
-      </c>
-      <c r="L85" t="inlineStr">
-        <is>
-          <t>92%</t>
-        </is>
-      </c>
-      <c r="M85" t="inlineStr">
         <is>
           <t>g147319-d23482969</t>
         </is>
@@ -5113,20 +4376,10 @@
       </c>
       <c r="J86" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K86" t="inlineStr">
-        <is>
-          <t>Villa Herencia Hotel</t>
-        </is>
-      </c>
-      <c r="L86" t="inlineStr">
-        <is>
-          <t>61%</t>
-        </is>
-      </c>
-      <c r="M86" t="inlineStr">
         <is>
           <t>g147319-d1048165</t>
         </is>
@@ -5169,16 +4422,6 @@
       </c>
       <c r="K87" t="inlineStr">
         <is>
-          <t>Hix Island House</t>
-        </is>
-      </c>
-      <c r="L87" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M87" t="inlineStr">
-        <is>
           <t>g147319-d147790</t>
         </is>
       </c>
@@ -5211,7 +4454,7 @@
         <v>202512</v>
       </c>
       <c r="I88" t="n">
-        <v>237</v>
+        <v>242</v>
       </c>
       <c r="J88" t="inlineStr">
         <is>
@@ -5219,16 +4462,6 @@
         </is>
       </c>
       <c r="K88" t="inlineStr">
-        <is>
-          <t>Park Royal Homestay Club Cala Puerto Rico</t>
-        </is>
-      </c>
-      <c r="L88" t="inlineStr">
-        <is>
-          <t>83%</t>
-        </is>
-      </c>
-      <c r="M88" t="inlineStr">
         <is>
           <t>g147319-d6161031</t>
         </is>
@@ -5263,20 +4496,10 @@
       </c>
       <c r="J89" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K89" t="inlineStr">
-        <is>
-          <t>Casa Verde Hotel</t>
-        </is>
-      </c>
-      <c r="L89" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M89" t="inlineStr">
         <is>
           <t>g147319-d668014</t>
         </is>
@@ -5310,7 +4533,7 @@
         <v>202512</v>
       </c>
       <c r="I90" t="n">
-        <v>403</v>
+        <v>427</v>
       </c>
       <c r="J90" t="inlineStr">
         <is>
@@ -5318,16 +4541,6 @@
         </is>
       </c>
       <c r="K90" t="inlineStr">
-        <is>
-          <t>Holiday Inn Express San Juan Condado by IHG</t>
-        </is>
-      </c>
-      <c r="L90" t="inlineStr">
-        <is>
-          <t>90%</t>
-        </is>
-      </c>
-      <c r="M90" t="inlineStr">
         <is>
           <t>g147319-d151941</t>
         </is>
@@ -5370,16 +4583,6 @@
       </c>
       <c r="K91" t="inlineStr">
         <is>
-          <t>Hotel Nest</t>
-        </is>
-      </c>
-      <c r="L91" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M91" t="inlineStr">
-        <is>
           <t>g147319-d23865228</t>
         </is>
       </c>
@@ -5413,7 +4616,12 @@
       </c>
       <c r="J92" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K92" t="inlineStr">
+        <is>
+          <t>g609121-d60096</t>
         </is>
       </c>
     </row>
@@ -5446,20 +4654,10 @@
       </c>
       <c r="J93" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K93" t="inlineStr">
-        <is>
-          <t>CasaBlanca Hotel</t>
-        </is>
-      </c>
-      <c r="L93" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M93" t="inlineStr">
         <is>
           <t>g147319-d1456033</t>
         </is>
@@ -5493,24 +4691,14 @@
         <v>202512</v>
       </c>
       <c r="I94" t="n">
-        <v>91</v>
+        <v>126</v>
       </c>
       <c r="J94" t="inlineStr">
         <is>
-          <t>Agoda.com</t>
+          <t>Vio.com</t>
         </is>
       </c>
       <c r="K94" t="inlineStr">
-        <is>
-          <t>Dreams Hotel Puerto Rico</t>
-        </is>
-      </c>
-      <c r="L94" t="inlineStr">
-        <is>
-          <t>97%</t>
-        </is>
-      </c>
-      <c r="M94" t="inlineStr">
         <is>
           <t>g147319-d2481661</t>
         </is>
@@ -5553,16 +4741,6 @@
       </c>
       <c r="K95" t="inlineStr">
         <is>
-          <t>Hosteria Del Mar</t>
-        </is>
-      </c>
-      <c r="L95" t="inlineStr">
-        <is>
-          <t>92%</t>
-        </is>
-      </c>
-      <c r="M95" t="inlineStr">
-        <is>
           <t>g147319-d148560</t>
         </is>
       </c>
@@ -5594,25 +4772,12 @@
       <c r="F96" t="n">
         <v>202512</v>
       </c>
-      <c r="I96" t="n">
-        <v>405</v>
-      </c>
       <c r="J96" t="inlineStr">
         <is>
-          <t>Trip.com</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K96" t="inlineStr">
-        <is>
-          <t>Caribe Hilton Hotel</t>
-        </is>
-      </c>
-      <c r="L96" t="inlineStr">
-        <is>
-          <t>72%</t>
-        </is>
-      </c>
-      <c r="M96" t="inlineStr">
         <is>
           <t>g147319-d149921</t>
         </is>
@@ -5645,11 +4810,6 @@
       <c r="F97" t="n">
         <v>202512</v>
       </c>
-      <c r="J97" t="inlineStr">
-        <is>
-          <t>Not found</t>
-        </is>
-      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -5688,16 +4848,6 @@
       </c>
       <c r="K98" t="inlineStr">
         <is>
-          <t>Hotel El Guajataca</t>
-        </is>
-      </c>
-      <c r="L98" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M98" t="inlineStr">
-        <is>
           <t>g147319-d150417</t>
         </is>
       </c>
@@ -5739,16 +4889,6 @@
       </c>
       <c r="K99" t="inlineStr">
         <is>
-          <t>Hotel Mayaguez Plaza, BW Signature Collection</t>
-        </is>
-      </c>
-      <c r="L99" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M99" t="inlineStr">
-        <is>
           <t>g147319-d575670</t>
         </is>
       </c>
@@ -5782,20 +4922,10 @@
       </c>
       <c r="J100" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K100" t="inlineStr">
-        <is>
-          <t>The Lazy Parrot Inn</t>
-        </is>
-      </c>
-      <c r="L100" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M100" t="inlineStr">
         <is>
           <t>g147319-d148789</t>
         </is>
@@ -5838,16 +4968,6 @@
       </c>
       <c r="K101" t="inlineStr">
         <is>
-          <t>Coral Princess Hotel</t>
-        </is>
-      </c>
-      <c r="L101" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M101" t="inlineStr">
-        <is>
           <t>g147319-d268429</t>
         </is>
       </c>
@@ -5889,16 +5009,6 @@
       </c>
       <c r="K102" t="inlineStr">
         <is>
-          <t>Dream Inn PR</t>
-        </is>
-      </c>
-      <c r="L102" t="inlineStr">
-        <is>
-          <t>80%</t>
-        </is>
-      </c>
-      <c r="M102" t="inlineStr">
-        <is>
           <t>g147319-d7316138</t>
         </is>
       </c>
@@ -5940,16 +5050,6 @@
       </c>
       <c r="K103" t="inlineStr">
         <is>
-          <t>Dreams Hotel Miramar</t>
-        </is>
-      </c>
-      <c r="L103" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M103" t="inlineStr">
-        <is>
           <t>g147319-d14943546</t>
         </is>
       </c>
@@ -5983,20 +5083,10 @@
       </c>
       <c r="J104" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K104" t="inlineStr">
-        <is>
-          <t>The Looking Glass Hotel</t>
-        </is>
-      </c>
-      <c r="L104" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M104" t="inlineStr">
         <is>
           <t>g147319-d27184349</t>
         </is>
@@ -6031,20 +5121,10 @@
       </c>
       <c r="J105" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K105" t="inlineStr">
-        <is>
-          <t>At Wind Chimes Boutique Hotel</t>
-        </is>
-      </c>
-      <c r="L105" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M105" t="inlineStr">
         <is>
           <t>g147319-d151679</t>
         </is>
@@ -6079,20 +5159,10 @@
       </c>
       <c r="J106" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K106" t="inlineStr">
-        <is>
-          <t>Hacienda Tamarindo</t>
-        </is>
-      </c>
-      <c r="L106" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M106" t="inlineStr">
         <is>
           <t>g147319-d147798</t>
         </is>
@@ -6127,20 +5197,10 @@
       </c>
       <c r="J107" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K107" t="inlineStr">
-        <is>
-          <t>Seagate Hotel</t>
-        </is>
-      </c>
-      <c r="L107" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M107" t="inlineStr">
         <is>
           <t>g147319-d485475</t>
         </is>
@@ -6173,25 +5233,12 @@
       <c r="F108" t="n">
         <v>202512</v>
       </c>
-      <c r="I108" t="n">
-        <v>118</v>
-      </c>
       <c r="J108" t="inlineStr">
         <is>
-          <t>Vio.com</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K108" t="inlineStr">
-        <is>
-          <t>Coconut Palms Inn</t>
-        </is>
-      </c>
-      <c r="L108" t="inlineStr">
-        <is>
-          <t>74%</t>
-        </is>
-      </c>
-      <c r="M108" t="inlineStr">
         <is>
           <t>g147319-d267552</t>
         </is>
@@ -6234,16 +5281,6 @@
       </c>
       <c r="K109" t="inlineStr">
         <is>
-          <t>Nautilus By La Jamaca Hotel - La Parguera</t>
-        </is>
-      </c>
-      <c r="L109" t="inlineStr">
-        <is>
-          <t>77%</t>
-        </is>
-      </c>
-      <c r="M109" t="inlineStr">
-        <is>
           <t>g147319-d3310458</t>
         </is>
       </c>
@@ -6277,20 +5314,10 @@
       </c>
       <c r="J110" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K110" t="inlineStr">
-        <is>
-          <t>Casa Resaca</t>
-        </is>
-      </c>
-      <c r="L110" t="inlineStr">
-        <is>
-          <t>62%</t>
-        </is>
-      </c>
-      <c r="M110" t="inlineStr">
         <is>
           <t>g147319-d2058980</t>
         </is>
@@ -6325,20 +5352,10 @@
       </c>
       <c r="J111" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K111" t="inlineStr">
-        <is>
-          <t>Hotel Punta Maracayo</t>
-        </is>
-      </c>
-      <c r="L111" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M111" t="inlineStr">
         <is>
           <t>g147319-d1391914</t>
         </is>
@@ -6372,7 +5389,7 @@
         <v>202512</v>
       </c>
       <c r="I112" t="n">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="J112" t="inlineStr">
         <is>
@@ -6380,16 +5397,6 @@
         </is>
       </c>
       <c r="K112" t="inlineStr">
-        <is>
-          <t>Costa Bahia Hotel &amp; Convention Center</t>
-        </is>
-      </c>
-      <c r="L112" t="inlineStr">
-        <is>
-          <t>95%</t>
-        </is>
-      </c>
-      <c r="M112" t="inlineStr">
         <is>
           <t>g147319-d251396</t>
         </is>
@@ -6424,20 +5431,10 @@
       </c>
       <c r="J113" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K113" t="inlineStr">
-        <is>
-          <t>Hacienda Gripinas</t>
-        </is>
-      </c>
-      <c r="L113" t="inlineStr">
-        <is>
-          <t>94%</t>
-        </is>
-      </c>
-      <c r="M113" t="inlineStr">
         <is>
           <t>g147319-d151668</t>
         </is>
@@ -6480,16 +5477,6 @@
       </c>
       <c r="K114" t="inlineStr">
         <is>
-          <t>Parador MaunaCaribe</t>
-        </is>
-      </c>
-      <c r="L114" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M114" t="inlineStr">
-        <is>
           <t>g147319-d1681896</t>
         </is>
       </c>
@@ -6523,20 +5510,10 @@
       </c>
       <c r="J115" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K115" t="inlineStr">
-        <is>
-          <t>The Serene House Bed &amp; Breakfast</t>
-        </is>
-      </c>
-      <c r="L115" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M115" t="inlineStr">
         <is>
           <t>g147319-d26723746</t>
         </is>
@@ -6571,20 +5548,10 @@
       </c>
       <c r="J116" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K116" t="inlineStr">
-        <is>
-          <t>Casa Sol Bed &amp; Breakfast</t>
-        </is>
-      </c>
-      <c r="L116" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M116" t="inlineStr">
         <is>
           <t>g147319-d5964475</t>
         </is>
@@ -6619,20 +5586,10 @@
       </c>
       <c r="J117" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K117" t="inlineStr">
-        <is>
-          <t>Parador Boquemar</t>
-        </is>
-      </c>
-      <c r="L117" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M117" t="inlineStr">
         <is>
           <t>g147319-d151667</t>
         </is>
@@ -6667,20 +5624,10 @@
       </c>
       <c r="J118" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K118" t="inlineStr">
-        <is>
-          <t>Parador Villa Parguera</t>
-        </is>
-      </c>
-      <c r="L118" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M118" t="inlineStr">
         <is>
           <t>g147319-d151670</t>
         </is>
@@ -6715,7 +5662,12 @@
       </c>
       <c r="J119" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>N/A</t>
+        </is>
+      </c>
+      <c r="K119" t="inlineStr">
+        <is>
+          <t>g147319-d293708</t>
         </is>
       </c>
     </row>
@@ -6756,16 +5708,6 @@
       </c>
       <c r="K120" t="inlineStr">
         <is>
-          <t>Ficus Hotel</t>
-        </is>
-      </c>
-      <c r="L120" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M120" t="inlineStr">
-        <is>
           <t>g147319-d25456741</t>
         </is>
       </c>
@@ -6799,20 +5741,10 @@
       </c>
       <c r="J121" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K121" t="inlineStr">
-        <is>
-          <t>Tapia Haus 103</t>
-        </is>
-      </c>
-      <c r="L121" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M121" t="inlineStr">
         <is>
           <t>g147319-d20243623</t>
         </is>
@@ -6846,24 +5778,14 @@
         <v>202512</v>
       </c>
       <c r="I122" t="n">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="J122" t="inlineStr">
         <is>
-          <t>Booking.com</t>
+          <t>Agoda.com</t>
         </is>
       </c>
       <c r="K122" t="inlineStr">
-        <is>
-          <t>Parador El Buen Cafe</t>
-        </is>
-      </c>
-      <c r="L122" t="inlineStr">
-        <is>
-          <t>65%</t>
-        </is>
-      </c>
-      <c r="M122" t="inlineStr">
         <is>
           <t>g147319-d251395</t>
         </is>
@@ -6898,20 +5820,10 @@
       </c>
       <c r="J123" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K123" t="inlineStr">
-        <is>
-          <t>Marina Real Apartments</t>
-        </is>
-      </c>
-      <c r="L123" t="inlineStr">
-        <is>
-          <t>61%</t>
-        </is>
-      </c>
-      <c r="M123" t="inlineStr">
         <is>
           <t>g147319-d2066940</t>
         </is>
@@ -6944,9 +5856,17 @@
       <c r="F124" t="n">
         <v>202512</v>
       </c>
+      <c r="I124" t="n">
+        <v>46</v>
+      </c>
       <c r="J124" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>Booking.com</t>
+        </is>
+      </c>
+      <c r="K124" t="inlineStr">
+        <is>
+          <t>g147319-d14920354</t>
         </is>
       </c>
     </row>
@@ -6979,20 +5899,10 @@
       </c>
       <c r="J125" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K125" t="inlineStr">
-        <is>
-          <t>Dos Angeles Del Mar Bed &amp; Breakfast</t>
-        </is>
-      </c>
-      <c r="L125" t="inlineStr">
-        <is>
-          <t>81%</t>
-        </is>
-      </c>
-      <c r="M125" t="inlineStr">
         <is>
           <t>g147319-d291146</t>
         </is>
@@ -7035,16 +5945,6 @@
       </c>
       <c r="K126" t="inlineStr">
         <is>
-          <t>Luquillo Sunrise Beach Inn</t>
-        </is>
-      </c>
-      <c r="L126" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M126" t="inlineStr">
-        <is>
           <t>g147319-d649104</t>
         </is>
       </c>
@@ -7078,20 +5978,10 @@
       </c>
       <c r="J127" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K127" t="inlineStr">
-        <is>
-          <t>Casa Isabel B&amp;B</t>
-        </is>
-      </c>
-      <c r="L127" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M127" t="inlineStr">
         <is>
           <t>g147319-d9463907</t>
         </is>
@@ -7126,20 +6016,10 @@
       </c>
       <c r="J128" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K128" t="inlineStr">
-        <is>
-          <t>Casa Campo Bed And Breakfast</t>
-        </is>
-      </c>
-      <c r="L128" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M128" t="inlineStr">
         <is>
           <t>g147319-d13373035</t>
         </is>
@@ -7172,9 +6052,17 @@
       <c r="F129" t="n">
         <v>202512</v>
       </c>
+      <c r="I129" t="n">
+        <v>156</v>
+      </c>
       <c r="J129" t="inlineStr">
         <is>
-          <t>Not found</t>
+          <t>Booking.com</t>
+        </is>
+      </c>
+      <c r="K129" t="inlineStr">
+        <is>
+          <t>g147319-d151966</t>
         </is>
       </c>
     </row>
@@ -7206,24 +6094,14 @@
         <v>202512</v>
       </c>
       <c r="I130" t="n">
-        <v>158</v>
+        <v>135</v>
       </c>
       <c r="J130" t="inlineStr">
         <is>
-          <t>Booking.com</t>
+          <t>Vio.com</t>
         </is>
       </c>
       <c r="K130" t="inlineStr">
-        <is>
-          <t>Parador El Faro</t>
-        </is>
-      </c>
-      <c r="L130" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M130" t="inlineStr">
         <is>
           <t>g147319-d268433</t>
         </is>
@@ -7257,24 +6135,14 @@
         <v>202512</v>
       </c>
       <c r="I131" t="n">
-        <v>166</v>
+        <v>137</v>
       </c>
       <c r="J131" t="inlineStr">
         <is>
-          <t>Booking.com</t>
+          <t>Vio.com</t>
         </is>
       </c>
       <c r="K131" t="inlineStr">
-        <is>
-          <t>Parador Guánica 1929</t>
-        </is>
-      </c>
-      <c r="L131" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M131" t="inlineStr">
         <is>
           <t>g147319-d590083</t>
         </is>
@@ -7308,7 +6176,7 @@
         <v>202512</v>
       </c>
       <c r="I132" t="n">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="J132" t="inlineStr">
         <is>
@@ -7316,16 +6184,6 @@
         </is>
       </c>
       <c r="K132" t="inlineStr">
-        <is>
-          <t>Posada Hotel Colonial</t>
-        </is>
-      </c>
-      <c r="L132" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M132" t="inlineStr">
         <is>
           <t>g147319-d1007145</t>
         </is>
@@ -7360,20 +6218,10 @@
       </c>
       <c r="J133" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K133" t="inlineStr">
-        <is>
-          <t>Rincon Plaza Hotel</t>
-        </is>
-      </c>
-      <c r="L133" t="inlineStr">
-        <is>
-          <t>92%</t>
-        </is>
-      </c>
-      <c r="M133" t="inlineStr">
         <is>
           <t>g147319-d10730993</t>
         </is>
@@ -7408,20 +6256,10 @@
       </c>
       <c r="J134" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K134" t="inlineStr">
-        <is>
-          <t>San Sebastian Bed &amp; Breakfast</t>
-        </is>
-      </c>
-      <c r="L134" t="inlineStr">
-        <is>
-          <t>96%</t>
-        </is>
-      </c>
-      <c r="M134" t="inlineStr">
         <is>
           <t>g147319-d7720672</t>
         </is>
@@ -7464,16 +6302,6 @@
       </c>
       <c r="K135" t="inlineStr">
         <is>
-          <t>The Village Inn Hotel</t>
-        </is>
-      </c>
-      <c r="L135" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M135" t="inlineStr">
-        <is>
           <t>g147319-d8522359</t>
         </is>
       </c>
@@ -7506,24 +6334,14 @@
         <v>202512</v>
       </c>
       <c r="I136" t="n">
-        <v>148</v>
+        <v>164</v>
       </c>
       <c r="J136" t="inlineStr">
         <is>
-          <t>Vio.com</t>
+          <t>Booking.com</t>
         </is>
       </c>
       <c r="K136" t="inlineStr">
-        <is>
-          <t>Villa Verde Inn</t>
-        </is>
-      </c>
-      <c r="L136" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M136" t="inlineStr">
         <is>
           <t>g147319-d267488</t>
         </is>
@@ -7558,20 +6376,10 @@
       </c>
       <c r="J137" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K137" t="inlineStr">
-        <is>
-          <t>Comfort Inn &amp; Suites</t>
-        </is>
-      </c>
-      <c r="L137" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M137" t="inlineStr">
         <is>
           <t>g147319-d1151081</t>
         </is>
@@ -7605,24 +6413,14 @@
         <v>202512</v>
       </c>
       <c r="I138" t="n">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="J138" t="inlineStr">
         <is>
-          <t>Agoda.com</t>
+          <t>Vio.com</t>
         </is>
       </c>
       <c r="K138" t="inlineStr">
-        <is>
-          <t>Canario Boutique Hotel</t>
-        </is>
-      </c>
-      <c r="L138" t="inlineStr">
-        <is>
-          <t>62%</t>
-        </is>
-      </c>
-      <c r="M138" t="inlineStr">
         <is>
           <t>g147319-d150242</t>
         </is>
@@ -7656,24 +6454,14 @@
         <v>202512</v>
       </c>
       <c r="I139" t="n">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="J139" t="inlineStr">
         <is>
-          <t>Agoda.com</t>
+          <t>Vio.com</t>
         </is>
       </c>
       <c r="K139" t="inlineStr">
-        <is>
-          <t>Canario Boutique Hotel</t>
-        </is>
-      </c>
-      <c r="L139" t="inlineStr">
-        <is>
-          <t>84%</t>
-        </is>
-      </c>
-      <c r="M139" t="inlineStr">
         <is>
           <t>g147319-d150242</t>
         </is>
@@ -7708,20 +6496,10 @@
       </c>
       <c r="J140" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K140" t="inlineStr">
-        <is>
-          <t>Hotel Media Luna</t>
-        </is>
-      </c>
-      <c r="L140" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M140" t="inlineStr">
         <is>
           <t>g147319-d7137980</t>
         </is>
@@ -7756,20 +6534,10 @@
       </c>
       <c r="J141" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K141" t="inlineStr">
-        <is>
-          <t>Dos Angeles Del Mar Bed &amp; Breakfast</t>
-        </is>
-      </c>
-      <c r="L141" t="inlineStr">
-        <is>
-          <t>97%</t>
-        </is>
-      </c>
-      <c r="M141" t="inlineStr">
         <is>
           <t>g147319-d291146</t>
         </is>
@@ -7804,20 +6572,10 @@
       </c>
       <c r="J142" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K142" t="inlineStr">
-        <is>
-          <t>Casa Isabel B&amp;B</t>
-        </is>
-      </c>
-      <c r="L142" t="inlineStr">
-        <is>
-          <t>77%</t>
-        </is>
-      </c>
-      <c r="M142" t="inlineStr">
         <is>
           <t>g147319-d9463907</t>
         </is>
@@ -7851,7 +6609,7 @@
         <v>202512</v>
       </c>
       <c r="I143" t="n">
-        <v>144</v>
+        <v>149</v>
       </c>
       <c r="J143" t="inlineStr">
         <is>
@@ -7859,16 +6617,6 @@
         </is>
       </c>
       <c r="K143" t="inlineStr">
-        <is>
-          <t>Turtle Bay Inn</t>
-        </is>
-      </c>
-      <c r="L143" t="inlineStr">
-        <is>
-          <t>71%</t>
-        </is>
-      </c>
-      <c r="M143" t="inlineStr">
         <is>
           <t>g147319-d1593115</t>
         </is>
@@ -7903,20 +6651,10 @@
       </c>
       <c r="J144" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K144" t="inlineStr">
-        <is>
-          <t>4 Casitas</t>
-        </is>
-      </c>
-      <c r="L144" t="inlineStr">
-        <is>
-          <t>100%</t>
-        </is>
-      </c>
-      <c r="M144" t="inlineStr">
         <is>
           <t>g147319-d15856029</t>
         </is>
@@ -7951,20 +6689,10 @@
       </c>
       <c r="J145" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K145" t="inlineStr">
-        <is>
-          <t>Hacienda Siesta Alegre</t>
-        </is>
-      </c>
-      <c r="L145" t="inlineStr">
-        <is>
-          <t>62%</t>
-        </is>
-      </c>
-      <c r="M145" t="inlineStr">
         <is>
           <t>g147319-d1984406</t>
         </is>
@@ -7997,11 +6725,6 @@
       <c r="F146" t="n">
         <v>202512</v>
       </c>
-      <c r="J146" t="inlineStr">
-        <is>
-          <t>Not found</t>
-        </is>
-      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -8032,20 +6755,10 @@
       </c>
       <c r="J147" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K147" t="inlineStr">
-        <is>
-          <t>Pitahaya Glamping</t>
-        </is>
-      </c>
-      <c r="L147" t="inlineStr">
-        <is>
-          <t>74%</t>
-        </is>
-      </c>
-      <c r="M147" t="inlineStr">
         <is>
           <t>g147319-d15585165</t>
         </is>
@@ -8080,20 +6793,10 @@
       </c>
       <c r="J148" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K148" t="inlineStr">
-        <is>
-          <t>Flamboyan Guest House</t>
-        </is>
-      </c>
-      <c r="L148" t="inlineStr">
-        <is>
-          <t>63%</t>
-        </is>
-      </c>
-      <c r="M148" t="inlineStr">
         <is>
           <t>g147319-d681285</t>
         </is>
@@ -8128,20 +6831,10 @@
       </c>
       <c r="J149" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K149" t="inlineStr">
-        <is>
-          <t>Casa Robinson Guest House</t>
-        </is>
-      </c>
-      <c r="L149" t="inlineStr">
-        <is>
-          <t>75%</t>
-        </is>
-      </c>
-      <c r="M149" t="inlineStr">
         <is>
           <t>g147319-d636068</t>
         </is>
@@ -8176,20 +6869,10 @@
       </c>
       <c r="J150" t="inlineStr">
         <is>
-          <t>No price available</t>
+          <t>N/A</t>
         </is>
       </c>
       <c r="K150" t="inlineStr">
-        <is>
-          <t>A 2 Tiempos AyS, Bed and Breakfast</t>
-        </is>
-      </c>
-      <c r="L150" t="inlineStr">
-        <is>
-          <t>98%</t>
-        </is>
-      </c>
-      <c r="M150" t="inlineStr">
         <is>
           <t>g147319-d14037453</t>
         </is>
@@ -8232,16 +6915,6 @@
       </c>
       <c r="K151" t="inlineStr">
         <is>
-          <t>Conturce Hostel</t>
-        </is>
-      </c>
-      <c r="L151" t="inlineStr">
-        <is>
-          <t>77%</t>
-        </is>
-      </c>
-      <c r="M151" t="inlineStr">
-        <is>
           <t>g147319-d12379060</t>
         </is>
       </c>
@@ -8282,16 +6955,6 @@
         </is>
       </c>
       <c r="K152" t="inlineStr">
-        <is>
-          <t>Nomada Urban Beach Hostel - Calle Loiza</t>
-        </is>
-      </c>
-      <c r="L152" t="inlineStr">
-        <is>
-          <t>97%</t>
-        </is>
-      </c>
-      <c r="M152" t="inlineStr">
         <is>
           <t>g147319-d12640390</t>
         </is>

</xml_diff>